<commit_message>
overhauled project, including new pdf to txt conversion
</commit_message>
<xml_diff>
--- a/htm_links.xlsx
+++ b/htm_links.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\14a_background_scraper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D43752D-6180-4A8F-9F9F-3F741957C753}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2D1E476-2B23-493A-9018-CDDFB5B921FC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{20861DB0-DBCD-412B-9F60-CC7961AC5509}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{20861DB0-DBCD-412B-9F60-CC7961AC5509}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>https://www.sec.gov/Archives/edgar/data/1062613/000104746917000993/a2231072zdefm14a.htm</t>
   </si>
@@ -49,16 +49,30 @@
   </si>
   <si>
     <t>file</t>
+  </si>
+  <si>
+    <t>https://www.sec.gov/Archives/edgar/data/1037760/000119312516733208/d263126ddefm14a.htm</t>
+  </si>
+  <si>
+    <t>https://www.sec.gov/Archives/edgar/data/1226308/000119312516744017/d215313ddefm14a.htm</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -81,13 +95,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -400,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{836D8C61-43EB-4A27-AF6F-7CE820FB1C23}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -417,7 +434,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
@@ -432,7 +449,20 @@
         <v>3</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{C720B49B-1FF5-4B9E-89FD-D9B9C8F12F44}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>